<commit_message>
[data-raw] Inclusion of smoking attributable tables.
</commit_message>
<xml_diff>
--- a/data-raw/srelrisk_lus.xlsx
+++ b/data-raw/srelrisk_lus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Public Work UNRESTRICTED\Tasks\aafractions.ncc\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100010_{E4D25A77-AA39-41DD-8891-AF7B49778079}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100010_{C86D5D15-1614-4BF1-A02D-692BD3151DA4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18945" yWindow="450" windowWidth="13095" windowHeight="10200" tabRatio="699" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="13095" windowHeight="7770" tabRatio="699" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -210,20 +210,6 @@
     <t>C67</t>
   </si>
   <si>
-    <r>
-      <t>Kidney and Renal Pelvis</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
     <t>C64-C66,C68</t>
   </si>
   <si>
@@ -239,35 +225,7 @@
     <t>C25</t>
   </si>
   <si>
-    <r>
-      <t>Unspecified site</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
     <t>C80</t>
-  </si>
-  <si>
-    <r>
-      <t>Myeloid leukaemia</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
   </si>
   <si>
     <t>C92</t>
@@ -673,6 +631,15 @@
   <si>
     <t>ex smokers</t>
   </si>
+  <si>
+    <t>Kidney and Renal Pelvis</t>
+  </si>
+  <si>
+    <t>Unspecified site</t>
+  </si>
+  <si>
+    <t>Myeloid leukaemia</t>
+  </si>
 </sst>
 </file>
 
@@ -682,7 +649,7 @@
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -744,12 +711,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -966,18 +927,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -993,19 +954,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="7" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="7" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="5" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1015,60 +976,60 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="21" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="20" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="12" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="12" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="12" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1085,14 +1046,14 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1115,10 +1076,10 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1152,17 +1113,17 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1176,14 +1137,14 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2568,23 +2529,23 @@
     </row>
     <row r="6" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -2592,25 +2553,25 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12" s="15"/>
     </row>
     <row r="13" spans="2:5" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="16"/>
     </row>
     <row r="15" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C15" s="14"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="18"/>
@@ -2624,7 +2585,7 @@
     </row>
     <row r="18" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="20"/>
@@ -2632,130 +2593,130 @@
     </row>
     <row r="19" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
     </row>
     <row r="20" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="21" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
     </row>
     <row r="21" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
     </row>
     <row r="22" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
     </row>
     <row r="23" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
     </row>
     <row r="24" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
     </row>
     <row r="25" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
     </row>
     <row r="26" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
     </row>
     <row r="27" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
     <row r="28" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="21" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
     </row>
     <row r="30" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="21" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
@@ -2767,7 +2728,7 @@
     </row>
     <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B33" s="29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="31"/>
@@ -2775,7 +2736,7 @@
     </row>
     <row r="34" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="33"/>
@@ -2783,27 +2744,27 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="32" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C35" s="32"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="32" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C36" s="32"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="32" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C38" s="32"/>
     </row>
@@ -2813,19 +2774,19 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C40" s="34"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C41" s="35"/>
     </row>
     <row r="42" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="36" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C42" s="36"/>
     </row>
@@ -2843,42 +2804,42 @@
     </row>
     <row r="46" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="38" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C46" s="38"/>
     </row>
     <row r="47" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C47" s="38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C48" s="39"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C49" s="17"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C50" s="17"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="40" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C51" s="39" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3005,16 +2966,16 @@
         <v>34</v>
       </c>
       <c r="B6" s="93" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C6" s="93" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D6" s="93" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E6" s="93" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F6" s="18"/>
     </row>
@@ -3339,8 +3300,8 @@
   </sheetPr>
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3427,7 +3388,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="82" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D6" s="83" t="s">
         <v>33</v>
@@ -3450,7 +3411,7 @@
     </row>
     <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="85" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B7" s="85" t="str">
         <f>B6</f>
@@ -3671,14 +3632,14 @@
         <f t="shared" si="0"/>
         <v>Cancers which can be caused by smoking</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="76">
+        <v>2</v>
+      </c>
+      <c r="D15" s="47" t="s">
         <v>51</v>
-      </c>
-      <c r="C15" s="50">
-        <v>2</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>52</v>
       </c>
       <c r="E15" s="47" t="s">
         <v>40</v>
@@ -3702,11 +3663,11 @@
         <v>Cancers which can be caused by smoking</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="50"/>
       <c r="D16" s="47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" s="47" t="s">
         <v>40</v>
@@ -3730,11 +3691,11 @@
         <v>Cancers which can be caused by smoking</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="50"/>
       <c r="D17" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="47" t="s">
         <v>40</v>
@@ -3757,14 +3718,14 @@
         <f t="shared" si="0"/>
         <v>Cancers which can be caused by smoking</v>
       </c>
-      <c r="B18" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="50">
+      <c r="B18" s="76" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="76">
         <v>2</v>
       </c>
       <c r="D18" s="47" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" s="47" t="s">
         <v>40</v>
@@ -3787,14 +3748,14 @@
         <f t="shared" si="0"/>
         <v>Cancers which can be caused by smoking</v>
       </c>
-      <c r="B19" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="50">
+      <c r="B19" s="76" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="76">
         <v>2</v>
       </c>
       <c r="D19" s="47" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E19" s="47" t="s">
         <v>40</v>
@@ -3825,7 +3786,7 @@
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="87" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B21" s="87"/>
       <c r="C21" s="46"/>
@@ -3842,11 +3803,11 @@
         <v>Respiratory diseases which can be caused by smoking</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C22" s="50"/>
       <c r="D22" s="47" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E22" s="47" t="s">
         <v>40</v>
@@ -3870,11 +3831,11 @@
         <v>Respiratory diseases which can be caused by smoking</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" s="52"/>
       <c r="D23" s="47" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E23" s="47" t="s">
         <v>40</v>
@@ -3898,16 +3859,16 @@
         <v>Respiratory diseases which can be caused by smoking</v>
       </c>
       <c r="B24" s="76" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C24" s="76">
         <v>2</v>
       </c>
       <c r="D24" s="47" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E24" s="47" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F24" s="48">
         <v>2.5</v>
@@ -3928,16 +3889,16 @@
         <v>Respiratory diseases which can be caused by smoking</v>
       </c>
       <c r="B25" s="76" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C25" s="76">
         <v>2</v>
       </c>
       <c r="D25" s="47" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F25" s="48">
         <v>2</v>
@@ -3965,7 +3926,7 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="87" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B27" s="87"/>
       <c r="C27" s="46"/>
@@ -3982,11 +3943,11 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B28" s="54" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C28" s="54"/>
       <c r="D28" s="55" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E28" s="47" t="s">
         <v>40</v>
@@ -4010,16 +3971,16 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B29" s="76" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C29" s="76">
         <v>2</v>
       </c>
       <c r="D29" s="47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E29" s="47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F29" s="48">
         <v>4.2</v>
@@ -4040,16 +4001,16 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B30" s="76" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C30" s="76">
         <v>2</v>
       </c>
       <c r="D30" s="47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E30" s="47" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F30" s="48">
         <v>2.5</v>
@@ -4070,16 +4031,16 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B31" s="76" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C31" s="76">
         <v>2</v>
       </c>
       <c r="D31" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="47" t="s">
         <v>72</v>
-      </c>
-      <c r="E31" s="47" t="s">
-        <v>75</v>
       </c>
       <c r="F31" s="48">
         <v>1.8</v>
@@ -4100,16 +4061,16 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B32" s="76" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C32" s="76">
         <v>2</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E32" s="47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F32" s="48">
         <v>1.4</v>
@@ -4130,11 +4091,11 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C33" s="50"/>
       <c r="D33" s="47" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E33" s="47" t="s">
         <v>40</v>
@@ -4158,16 +4119,16 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B34" s="76" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C34" s="76">
         <v>2</v>
       </c>
       <c r="D34" s="47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E34" s="47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F34" s="48">
         <v>4.4000000000000004</v>
@@ -4188,16 +4149,16 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B35" s="76" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C35" s="76">
         <v>2</v>
       </c>
       <c r="D35" s="47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E35" s="47" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F35" s="48">
         <v>3.1</v>
@@ -4218,16 +4179,16 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B36" s="76" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C36" s="76">
         <v>2</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E36" s="47" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F36" s="48">
         <v>2.2000000000000002</v>
@@ -4248,16 +4209,16 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B37" s="76" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C37" s="76">
         <v>2</v>
       </c>
       <c r="D37" s="47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E37" s="47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F37" s="48">
         <v>1.6</v>
@@ -4278,11 +4239,11 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C38" s="50"/>
       <c r="D38" s="47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E38" s="47" t="s">
         <v>40</v>
@@ -4306,11 +4267,11 @@
         <v>Circulatory diseases which can be caused by smoking</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C39" s="50"/>
       <c r="D39" s="47" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E39" s="47" t="s">
         <v>40</v>
@@ -4341,7 +4302,7 @@
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="88" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B41" s="89"/>
       <c r="C41" s="56"/>
@@ -4358,11 +4319,11 @@
         <v>Diseases of the digestive system which can be caused caused by smoking</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C42" s="51"/>
       <c r="D42" s="47" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E42" s="47" t="s">
         <v>40</v>
@@ -4386,13 +4347,13 @@
         <v>Diseases of the digestive system which can be caused caused by smoking</v>
       </c>
       <c r="B43" s="76" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C43" s="76">
         <v>3</v>
       </c>
       <c r="D43" s="47" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E43" s="47" t="s">
         <v>40</v>
@@ -4416,13 +4377,13 @@
         <v>Diseases of the digestive system which can be caused caused by smoking</v>
       </c>
       <c r="B44" s="76" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C44" s="76">
         <v>3</v>
       </c>
       <c r="D44" s="47" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E44" s="47" t="s">
         <v>40</v>
@@ -4453,7 +4414,7 @@
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="87" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B46" s="87"/>
       <c r="C46" s="46"/>
@@ -4470,16 +4431,16 @@
         <v>Other diseases which can be caused by smoking</v>
       </c>
       <c r="B47" s="76" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C47" s="76">
         <v>3</v>
       </c>
       <c r="D47" s="47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E47" s="47" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F47" s="48">
         <v>1.54</v>
@@ -4500,16 +4461,16 @@
         <v>Other diseases which can be caused by smoking</v>
       </c>
       <c r="B48" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="C48" s="76" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" s="77" t="s">
-        <v>169</v>
-      </c>
       <c r="E48" s="47" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F48" s="48">
         <v>1.17</v>
@@ -4530,16 +4491,16 @@
         <v>Other diseases which can be caused by smoking</v>
       </c>
       <c r="B49" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="C49" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="C49" s="76" t="s">
-        <v>168</v>
-      </c>
-      <c r="D49" s="77" t="s">
-        <v>169</v>
-      </c>
       <c r="E49" s="47" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F49" s="48">
         <v>1.41</v>
@@ -4560,16 +4521,16 @@
         <v>Other diseases which can be caused by smoking</v>
       </c>
       <c r="B50" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="C50" s="76" t="s">
-        <v>168</v>
-      </c>
-      <c r="D50" s="77" t="s">
-        <v>169</v>
-      </c>
       <c r="E50" s="47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F50" s="48">
         <v>1.76</v>
@@ -4590,13 +4551,13 @@
         <v>Other diseases which can be caused by smoking</v>
       </c>
       <c r="B51" s="76" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C51" s="76">
         <v>3</v>
       </c>
       <c r="D51" s="47" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E51" s="47" t="s">
         <v>40</v>
@@ -4633,7 +4594,7 @@
     <row r="54" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="60"/>
       <c r="B54" s="60" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C54" s="60"/>
       <c r="D54" s="47"/>
@@ -4670,7 +4631,7 @@
     <row r="57" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="41"/>
       <c r="B57" s="41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C57" s="41"/>
       <c r="D57" s="47"/>
@@ -4683,7 +4644,7 @@
     <row r="58" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="41"/>
       <c r="B58" s="41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C58" s="41"/>
       <c r="D58" s="47"/>
@@ -4696,7 +4657,7 @@
     <row r="59" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="41"/>
       <c r="B59" s="41" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C59" s="41"/>
       <c r="D59" s="47"/>
@@ -4709,7 +4670,7 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="41"/>
       <c r="B60" s="41" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C60" s="41"/>
       <c r="D60" s="41"/>
@@ -4733,7 +4694,7 @@
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="62"/>
       <c r="B62" s="62" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C62" s="62"/>
       <c r="D62" s="41"/>
@@ -4746,7 +4707,7 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="41"/>
       <c r="B63" s="41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C63" s="41"/>
       <c r="D63" s="41"/>
@@ -4759,7 +4720,7 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="41"/>
       <c r="B64" s="41" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C64" s="41"/>
       <c r="D64" s="41"/>
@@ -4783,7 +4744,7 @@
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="41"/>
       <c r="B66" s="41" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C66" s="41"/>
       <c r="D66" s="41"/>
@@ -4821,7 +4782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F831F7E-E642-4D51-B145-13F003379413}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -4829,35 +4790,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="74" t="s">
-        <v>157</v>
-      </c>
       <c r="C7" s="75" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D7" s="75" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E7" s="75" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F7" s="75" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G7" s="75" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="71" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B8" s="72"/>
       <c r="C8" s="73">
@@ -4872,7 +4833,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="71" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="72"/>
       <c r="C9" s="73">
@@ -4910,7 +4871,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="71" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B11" s="72"/>
       <c r="C11" s="73"/>
@@ -4929,7 +4890,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="71" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B12" s="72"/>
       <c r="C12" s="73"/>
@@ -4942,7 +4903,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="71" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13" s="72"/>
       <c r="C13" s="73"/>
@@ -4955,7 +4916,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="71" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" s="72"/>
       <c r="C14" s="73"/>
@@ -4970,7 +4931,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="71" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" s="72"/>
       <c r="C15" s="73"/>

</xml_diff>

<commit_message>
[data-raw] smoking: extract relrisk no fractions
 - use ageband loookup to explode overlaps to continuous
 - add smoking family to datasets
</commit_message>
<xml_diff>
--- a/data-raw/srelrisk_lus.xlsx
+++ b/data-raw/srelrisk_lus.xlsx
@@ -8,24 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Public Work UNRESTRICTED\Tasks\aafractions.ncc\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100010_{C86D5D15-1614-4BF1-A02D-692BD3151DA4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0100BA27-2AD1-43D4-945F-11280D541A6E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="13095" windowHeight="7770" tabRatio="699" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="13095" windowHeight="7770" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="4" r:id="rId2"/>
-    <sheet name="NHSD SOS2018 Contents" sheetId="15" r:id="rId3"/>
-    <sheet name="B1" sheetId="13" r:id="rId4"/>
-    <sheet name="B2" sheetId="14" r:id="rId5"/>
-    <sheet name="ab_sa_explode" sheetId="16" r:id="rId6"/>
+    <sheet name="NHSD SOS2018 Contents" sheetId="15" r:id="rId2"/>
+    <sheet name="B1" sheetId="13" r:id="rId3"/>
+    <sheet name="B2" sheetId="14" r:id="rId4"/>
+    <sheet name="ab_sa_explode" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'B2'!$E$9:$E$51</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="4">ab_sa_explode!$A$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'B2'!$G$9:$G$51</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="3">ab_sa_explode!$A$8</definedName>
     <definedName name="HTML_CodePage" hidden="1">1252</definedName>
-    <definedName name="HTML_Control" localSheetId="4" hidden="1">{"'Trust by name'!$A$6:$E$350","'Trust by name'!$A$1:$D$348"}</definedName>
-    <definedName name="HTML_Control" localSheetId="2" hidden="1">{"'Trust by name'!$A$6:$E$350","'Trust by name'!$A$1:$D$348"}</definedName>
+    <definedName name="HTML_Control" localSheetId="3" hidden="1">{"'Trust by name'!$A$6:$E$350","'Trust by name'!$A$1:$D$348"}</definedName>
+    <definedName name="HTML_Control" localSheetId="1" hidden="1">{"'Trust by name'!$A$6:$E$350","'Trust by name'!$A$1:$D$348"}</definedName>
     <definedName name="HTML_Control" hidden="1">{"'Trust by name'!$A$6:$E$350","'Trust by name'!$A$1:$D$348"}</definedName>
     <definedName name="HTML_Description" hidden="1">""</definedName>
     <definedName name="HTML_Email" hidden="1">""</definedName>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="177">
   <si>
     <t>Prepared by:</t>
   </si>
@@ -575,9 +574,6 @@
     <t>psi@nationalarchives.gsi.gov.uk</t>
   </si>
   <si>
-    <t>ab_sa_explode</t>
-  </si>
-  <si>
     <t>35 - 44</t>
   </si>
   <si>
@@ -639,6 +635,21 @@
   </si>
   <si>
     <t>Myeloid leukaemia</t>
+  </si>
+  <si>
+    <t>ab_sa</t>
+  </si>
+  <si>
+    <t>analysis_type</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>morbidity</t>
+  </si>
+  <si>
+    <t>cat2</t>
   </si>
 </sst>
 </file>
@@ -680,6 +691,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -963,9 +975,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1017,18 +1026,6 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1045,9 +1042,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1080,12 +1074,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1126,12 +1114,6 @@
     <xf numFmtId="0" fontId="29" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1152,6 +1134,36 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -2003,13 +2015,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>889000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>876363</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>719666</xdr:rowOff>
@@ -2058,7 +2070,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{99B5941B-E009-4CE7-BC40-F928E91F4AF9}" name="Table1" displayName="Table1" ref="A7:G15" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A7:G15" xr:uid="{12DD428F-6CFE-4CC4-B9E1-653B3476B5D9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E68ED686-F425-4820-8CF7-4EA69D94604B}" name="ab_sa_explode" dataDxfId="6" dataCellStyle="Normal 5 2"/>
+    <tableColumn id="1" xr3:uid="{E68ED686-F425-4820-8CF7-4EA69D94604B}" name="ab_sa" dataDxfId="6" dataCellStyle="Normal 5 2"/>
     <tableColumn id="2" xr3:uid="{1004065E-4F79-4CD5-8B79-0A3AA721B125}" name="00 - 34" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{776FE795-26F3-48F1-A847-0774FAB5AB6A}" name="35 - 44" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{F9854AF2-85BC-4906-9852-E5D41F14BFC6}" name="45 - 54" dataDxfId="3"/>
@@ -2410,7 +2422,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <f ca="1">TODAY()</f>
-        <v>43528</v>
+        <v>43529</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2494,20 +2506,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <picture r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95639B1-33D4-4DD1-8034-1450CE6E6E18}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2558,10 +2556,10 @@
       <c r="C12" s="15"/>
     </row>
     <row r="13" spans="2:5" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="90"/>
     </row>
     <row r="15" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
@@ -2570,275 +2568,275 @@
       <c r="C15" s="14"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>107</v>
       </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="2:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
     </row>
     <row r="24" spans="2:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
     </row>
     <row r="25" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="26" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
     </row>
     <row r="27" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
     </row>
     <row r="28" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
     </row>
     <row r="30" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
     </row>
     <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
     </row>
     <row r="34" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="32"/>
+      <c r="C35" s="31"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="C36" s="32"/>
+      <c r="C36" s="31"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="C37" s="31" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="C38" s="32"/>
+      <c r="C38" s="31"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="34"/>
+      <c r="C40" s="33"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="C41" s="35"/>
+      <c r="C41" s="34"/>
     </row>
     <row r="42" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="91" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="36"/>
+      <c r="C42" s="91"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
+      <c r="B43" s="92"/>
+      <c r="C43" s="92"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
+      <c r="B44" s="92"/>
+      <c r="C44" s="92"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
+      <c r="B45" s="92"/>
+      <c r="C45" s="92"/>
     </row>
     <row r="46" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="C46" s="38"/>
+      <c r="C46" s="89"/>
     </row>
     <row r="47" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="89" t="s">
         <v>145</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="89" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="C48" s="39"/>
+      <c r="C48" s="35"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C49" s="17"/>
+      <c r="C49" s="16"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C50" s="17"/>
+      <c r="C50" s="16"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="C51" s="35" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2886,16 +2884,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEDE1F9-F115-4FF3-AC0C-2F0AD0FDB72F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2908,379 +2904,379 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="66" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="90"/>
-      <c r="B5" s="91" t="s">
+      <c r="A5" s="81"/>
+      <c r="B5" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="D5" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="18"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="84" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="84" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="93" t="s">
-        <v>169</v>
-      </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="84" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="84" t="s">
         <v>168</v>
       </c>
-      <c r="E6" s="93" t="s">
-        <v>169</v>
-      </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="str">
+      <c r="A7" s="85" t="str">
         <f>A6</f>
         <v>Age</v>
       </c>
-      <c r="B7" s="95" t="str">
+      <c r="B7" s="86" t="str">
         <f>B5 &amp; ";" &amp; B6</f>
         <v>Men;current smokers</v>
       </c>
-      <c r="C7" s="95" t="str">
+      <c r="C7" s="86" t="str">
         <f>C5 &amp; ";" &amp; C6</f>
         <v>Men;ex smokers</v>
       </c>
-      <c r="D7" s="95" t="str">
+      <c r="D7" s="86" t="str">
         <f>D5 &amp; ";" &amp; D6</f>
         <v>Women;current smokers</v>
       </c>
-      <c r="E7" s="95" t="str">
+      <c r="E7" s="86" t="str">
         <f>E5 &amp; ";" &amp; E6</f>
         <v>Women;ex smokers</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="68">
+      <c r="B8" s="61">
         <v>0.153</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="61">
         <v>0.35499999999999998</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="61">
         <v>0.122</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="61">
         <v>0.27600000000000002</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="61">
         <v>0.13700000000000001</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="61">
         <v>0.38900000000000001</v>
       </c>
-      <c r="D9" s="68">
+      <c r="D9" s="61">
         <v>0.115</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="61">
         <v>0.28899999999999998</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="67"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="18"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="68">
+      <c r="B11" s="61">
         <v>0.19500000000000001</v>
       </c>
-      <c r="C11" s="68">
+      <c r="C11" s="61">
         <v>0.25700000000000001</v>
       </c>
-      <c r="D11" s="68">
+      <c r="D11" s="61">
         <v>0.15</v>
       </c>
-      <c r="E11" s="68">
+      <c r="E11" s="61">
         <v>0.22700000000000001</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="68">
+      <c r="B12" s="61">
         <v>0.154</v>
       </c>
-      <c r="C12" s="68">
+      <c r="C12" s="61">
         <v>0.34399999999999997</v>
       </c>
-      <c r="D12" s="68">
+      <c r="D12" s="61">
         <v>0.13500000000000001</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="61">
         <v>0.27800000000000002</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="68">
+      <c r="B13" s="61">
         <v>0.106</v>
       </c>
-      <c r="C13" s="68">
+      <c r="C13" s="61">
         <v>0.49</v>
       </c>
-      <c r="D13" s="68">
+      <c r="D13" s="61">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="E13" s="68">
+      <c r="E13" s="61">
         <v>0.35299999999999998</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="68">
+      <c r="B14" s="61">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="C14" s="68">
+      <c r="C14" s="61">
         <v>0.56799999999999995</v>
       </c>
-      <c r="D14" s="68">
+      <c r="D14" s="61">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="E14" s="68">
+      <c r="E14" s="61">
         <v>0.33300000000000002</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="18"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="68">
+      <c r="B16" s="61">
         <v>0.182</v>
       </c>
-      <c r="C16" s="68">
+      <c r="C16" s="61">
         <v>0.28399999999999997</v>
       </c>
-      <c r="D16" s="68">
+      <c r="D16" s="61">
         <v>0.14499999999999999</v>
       </c>
-      <c r="E16" s="68">
+      <c r="E16" s="61">
         <v>0.24299999999999999</v>
       </c>
-      <c r="F16" s="18"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="67" t="s">
+      <c r="A17" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="68">
+      <c r="B17" s="61">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C17" s="68">
+      <c r="C17" s="61">
         <v>0.52200000000000002</v>
       </c>
-      <c r="D17" s="68">
+      <c r="D17" s="61">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="E17" s="68">
+      <c r="E17" s="61">
         <v>0.34399999999999997</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="69"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="18"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="62" t="s">
+      <c r="A26" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3293,1483 +3289,1853 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF3EE9FA-D003-4CB4-A71B-48BE9827B82C}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="8" customWidth="1"/>
-    <col min="5" max="5" width="10" style="8" customWidth="1"/>
-    <col min="6" max="9" width="13.42578125" style="8" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="3" width="16.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="8" customWidth="1"/>
+    <col min="7" max="7" width="10" style="8" customWidth="1"/>
+    <col min="8" max="11" width="13.42578125" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42" t="s">
+    <row r="1" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44" t="s">
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="78"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="80" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="71"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="80" t="s">
+      <c r="I5" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="80" t="s">
+      <c r="J5" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="80" t="s">
+      <c r="K5" s="73" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="81"/>
-      <c r="B6" s="81" t="s">
+    <row r="6" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="74"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="82" t="s">
+      <c r="E6" s="75" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="77" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="77" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="77" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="87" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="87" t="str">
+        <f>D6</f>
+        <v>Disease category</v>
+      </c>
+      <c r="E7" s="87" t="str">
+        <f>E6</f>
+        <v>Footnote</v>
+      </c>
+      <c r="F7" s="87" t="str">
+        <f>F6</f>
+        <v>ICD-10 code</v>
+      </c>
+      <c r="G7" s="87" t="str">
+        <f>G6</f>
+        <v>Age</v>
+      </c>
+      <c r="H7" s="88" t="str">
+        <f>H5 &amp; ";" &amp; H6</f>
+        <v>Men;Current smokers</v>
+      </c>
+      <c r="I7" s="88" t="str">
+        <f>I5 &amp; ";" &amp; I6</f>
+        <v>Men;Ex-smokers</v>
+      </c>
+      <c r="J7" s="88" t="str">
+        <f>J5 &amp; ";" &amp; J6</f>
+        <v>Women;Current smokers</v>
+      </c>
+      <c r="K7" s="88" t="str">
+        <f>K5 &amp; ";" &amp; K6</f>
+        <v>Women;Ex-smokers</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="78" t="str">
+        <f>IF(A8 = "all", "fatal", IF(LEN(A8) &gt; 0, "non-fatal", ""))</f>
+        <v>fatal</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="78"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+    </row>
+    <row r="9" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="69" t="str">
+        <f>A8</f>
+        <v>all</v>
+      </c>
+      <c r="B9" s="69" t="str">
+        <f t="shared" ref="B9:B51" si="0">IF(A9 = "all", "fatal", IF(LEN(A9) &gt; 0, "non-fatal", ""))</f>
+        <v>fatal</v>
+      </c>
+      <c r="C9" s="69" t="str">
+        <f>C8</f>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="45"/>
+      <c r="F9" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="43">
+        <v>23.26</v>
+      </c>
+      <c r="I9" s="43">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J9" s="43">
+        <v>12.69</v>
+      </c>
+      <c r="K9" s="43">
+        <v>4.53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="69" t="str">
+        <f t="shared" ref="A10:A50" si="1">A9</f>
+        <v>all</v>
+      </c>
+      <c r="B10" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C10" s="69" t="str">
+        <f t="shared" ref="C10:C19" si="2">C9</f>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="45"/>
+      <c r="F10" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="43">
+        <v>10.89</v>
+      </c>
+      <c r="I10" s="43">
+        <v>3.4</v>
+      </c>
+      <c r="J10" s="43">
+        <v>5.08</v>
+      </c>
+      <c r="K10" s="43">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B11" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C11" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="45"/>
+      <c r="F11" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="43">
+        <v>6.76</v>
+      </c>
+      <c r="I11" s="43">
+        <v>4.46</v>
+      </c>
+      <c r="J11" s="43">
+        <v>7.75</v>
+      </c>
+      <c r="K11" s="43">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B12" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C12" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="46"/>
+      <c r="F12" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="43">
+        <v>14.6</v>
+      </c>
+      <c r="I12" s="43">
+        <v>6.34</v>
+      </c>
+      <c r="J12" s="43">
+        <v>13.02</v>
+      </c>
+      <c r="K12" s="43">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B13" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C13" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="45"/>
+      <c r="F13" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="43">
+        <v>1</v>
+      </c>
+      <c r="I13" s="43">
+        <v>1</v>
+      </c>
+      <c r="J13" s="43">
+        <v>1.59</v>
+      </c>
+      <c r="K13" s="43">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B14" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C14" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="45"/>
+      <c r="F14" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="43">
+        <v>3.27</v>
+      </c>
+      <c r="I14" s="43">
+        <v>2.09</v>
+      </c>
+      <c r="J14" s="43">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="K14" s="43">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B15" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C15" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D15" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="69">
+        <v>2</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="I15" s="43">
+        <v>1.7</v>
+      </c>
+      <c r="J15" s="43">
+        <v>1.4</v>
+      </c>
+      <c r="K15" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B16" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C16" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="43">
+        <v>1.96</v>
+      </c>
+      <c r="I16" s="43">
+        <v>1.47</v>
+      </c>
+      <c r="J16" s="43">
+        <v>1.36</v>
+      </c>
+      <c r="K16" s="43">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B17" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C17" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="45"/>
+      <c r="F17" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="43">
+        <v>2.31</v>
+      </c>
+      <c r="I17" s="43">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J17" s="43">
+        <v>2.25</v>
+      </c>
+      <c r="K17" s="43">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B18" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C18" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D18" s="69" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="69">
+        <v>2</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="43">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I18" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="J18" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K18" s="43">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B19" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C19" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v>Cancers which can be caused by smoking</v>
+      </c>
+      <c r="D19" s="69" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="69">
+        <v>2</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="43">
+        <v>1.8</v>
+      </c>
+      <c r="I19" s="43">
+        <v>1.4</v>
+      </c>
+      <c r="J19" s="43">
+        <v>1.2</v>
+      </c>
+      <c r="K19" s="43">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="45"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="78" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C21" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="78"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
+    </row>
+    <row r="22" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B22" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C22" s="69" t="str">
+        <f t="shared" ref="C22:C25" si="3">C21</f>
+        <v>Respiratory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="45"/>
+      <c r="F22" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="43">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="I22" s="43">
+        <v>15.64</v>
+      </c>
+      <c r="J22" s="43">
+        <v>12.04</v>
+      </c>
+      <c r="K22" s="43">
+        <v>11.77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B23" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C23" s="69" t="str">
+        <f t="shared" si="3"/>
+        <v>Respiratory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="47"/>
+      <c r="F23" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="43">
+        <v>10.58</v>
+      </c>
+      <c r="I23" s="43">
+        <v>6.8</v>
+      </c>
+      <c r="J23" s="43">
+        <v>13.08</v>
+      </c>
+      <c r="K23" s="43">
+        <v>6.78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B24" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C24" s="69" t="str">
+        <f t="shared" si="3"/>
+        <v>Respiratory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D24" s="69" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="69">
+        <v>2</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="I24" s="43">
+        <v>1.4</v>
+      </c>
+      <c r="J24" s="43">
+        <v>4.3</v>
+      </c>
+      <c r="K24" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B25" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C25" s="69" t="str">
+        <f t="shared" si="3"/>
+        <v>Respiratory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D25" s="69" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" s="69">
+        <v>2</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="43">
+        <v>2</v>
+      </c>
+      <c r="I25" s="43">
+        <v>1.4</v>
+      </c>
+      <c r="J25" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K25" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="45"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+    </row>
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B27" s="78" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="78"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="43"/>
+    </row>
+    <row r="28" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B28" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C28" s="69" t="str">
+        <f t="shared" ref="C28:C39" si="4">C27</f>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="43">
+        <v>1.78</v>
+      </c>
+      <c r="I28" s="43">
+        <v>1.22</v>
+      </c>
+      <c r="J28" s="43">
+        <v>1.49</v>
+      </c>
+      <c r="K28" s="43">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B29" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C29" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D29" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="E29" s="69">
+        <v>2</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="43">
+        <v>4.2</v>
+      </c>
+      <c r="I29" s="43">
+        <v>2</v>
+      </c>
+      <c r="J29" s="43">
+        <v>5.3</v>
+      </c>
+      <c r="K29" s="43">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B30" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C30" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D30" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="69">
+        <v>2</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="I30" s="43">
+        <v>1.6</v>
+      </c>
+      <c r="J30" s="43">
+        <v>2.8</v>
+      </c>
+      <c r="K30" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B31" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C31" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D31" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" s="69">
+        <v>2</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="43">
+        <v>1.8</v>
+      </c>
+      <c r="I31" s="43">
+        <v>1.3</v>
+      </c>
+      <c r="J31" s="43">
+        <v>2.1</v>
+      </c>
+      <c r="K31" s="43">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B32" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C32" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D32" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="69">
+        <v>2</v>
+      </c>
+      <c r="F32" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="43">
+        <v>1.4</v>
+      </c>
+      <c r="I32" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J32" s="43">
+        <v>1.4</v>
+      </c>
+      <c r="K32" s="43">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B33" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C33" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D33" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="45"/>
+      <c r="F33" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="43">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="I33" s="43">
+        <v>1.01</v>
+      </c>
+      <c r="J33" s="43">
+        <v>2.17</v>
+      </c>
+      <c r="K33" s="43">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B34" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C34" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D34" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="84" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="84" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="85" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="85" t="str">
-        <f>B6</f>
-        <v>Disease category</v>
-      </c>
-      <c r="C7" s="85" t="str">
-        <f>C6</f>
-        <v>Footnote</v>
-      </c>
-      <c r="D7" s="85" t="str">
-        <f>D6</f>
-        <v>ICD-10 code</v>
-      </c>
-      <c r="E7" s="85" t="str">
-        <f>E6</f>
-        <v>Age</v>
-      </c>
-      <c r="F7" s="86" t="str">
-        <f>F5 &amp; ";" &amp; F6</f>
-        <v>Men;Current smokers</v>
-      </c>
-      <c r="G7" s="86" t="str">
-        <f>G5 &amp; ";" &amp; G6</f>
-        <v>Men;Ex-smokers</v>
-      </c>
-      <c r="H7" s="86" t="str">
-        <f>H5 &amp; ";" &amp; H6</f>
-        <v>Women;Current smokers</v>
-      </c>
-      <c r="I7" s="86" t="str">
-        <f>I5 &amp; ";" &amp; I6</f>
-        <v>Women;Ex-smokers</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-    </row>
-    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="76" t="str">
-        <f>A8</f>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="47" t="s">
+      <c r="E34" s="69">
+        <v>2</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" s="43">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I34" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J34" s="43">
+        <v>5.4</v>
+      </c>
+      <c r="K34" s="43">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B35" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C35" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D35" s="69" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="69">
+        <v>2</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" s="43">
+        <v>3.1</v>
+      </c>
+      <c r="I35" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J35" s="43">
+        <v>3.7</v>
+      </c>
+      <c r="K35" s="43">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A36" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B36" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C36" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D36" s="69" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="69">
+        <v>2</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I36" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J36" s="43">
+        <v>2.6</v>
+      </c>
+      <c r="K36" s="43">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B37" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C37" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D37" s="69" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="69">
+        <v>2</v>
+      </c>
+      <c r="F37" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" s="43">
+        <v>1.6</v>
+      </c>
+      <c r="I37" s="43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J37" s="43">
+        <v>1.3</v>
+      </c>
+      <c r="K37" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A38" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B38" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C38" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D38" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="45"/>
+      <c r="F38" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="48">
-        <v>23.26</v>
-      </c>
-      <c r="G9" s="48">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="H9" s="48">
-        <v>12.69</v>
-      </c>
-      <c r="I9" s="48">
-        <v>4.53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="76" t="str">
-        <f t="shared" ref="A10:A19" si="0">A9</f>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="47" t="s">
+      <c r="H38" s="43">
+        <v>6.21</v>
+      </c>
+      <c r="I38" s="43">
+        <v>3.07</v>
+      </c>
+      <c r="J38" s="43">
+        <v>7.07</v>
+      </c>
+      <c r="K38" s="43">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B39" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C39" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v>Circulatory diseases which can be caused by smoking</v>
+      </c>
+      <c r="D39" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="45"/>
+      <c r="F39" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="48">
-        <v>10.89</v>
-      </c>
-      <c r="G10" s="48">
-        <v>3.4</v>
-      </c>
-      <c r="H10" s="48">
-        <v>5.08</v>
-      </c>
-      <c r="I10" s="48">
-        <v>2.29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="76" t="str">
+      <c r="H39" s="43">
+        <v>2.44</v>
+      </c>
+      <c r="I39" s="43">
+        <v>1.33</v>
+      </c>
+      <c r="J39" s="43">
+        <v>1.83</v>
+      </c>
+      <c r="K39" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="45"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="43"/>
+    </row>
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" s="78" t="str">
         <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="47" t="s">
+        <v>fatal</v>
+      </c>
+      <c r="C41" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="80"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+    </row>
+    <row r="42" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>all</v>
+      </c>
+      <c r="B42" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>fatal</v>
+      </c>
+      <c r="C42" s="69" t="str">
+        <f t="shared" ref="C42:C44" si="5">C41</f>
+        <v>Diseases of the digestive system which can be caused caused by smoking</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" s="46"/>
+      <c r="F42" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="48">
-        <v>6.76</v>
-      </c>
-      <c r="G11" s="48">
-        <v>4.46</v>
-      </c>
-      <c r="H11" s="48">
-        <v>7.75</v>
-      </c>
-      <c r="I11" s="48">
-        <v>2.79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="76" t="str">
+      <c r="H42" s="43">
+        <v>5.4</v>
+      </c>
+      <c r="I42" s="43">
+        <v>1.8</v>
+      </c>
+      <c r="J42" s="43">
+        <v>5.5</v>
+      </c>
+      <c r="K42" s="43">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="78" t="str">
         <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B12" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="47" t="s">
+        <v>non-fatal</v>
+      </c>
+      <c r="C43" s="69" t="str">
+        <f t="shared" si="5"/>
+        <v>Diseases of the digestive system which can be caused caused by smoking</v>
+      </c>
+      <c r="D43" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="69">
+        <v>3</v>
+      </c>
+      <c r="F43" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="G43" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="48">
-        <v>14.6</v>
-      </c>
-      <c r="G12" s="48">
-        <v>6.34</v>
-      </c>
-      <c r="H12" s="48">
-        <v>13.02</v>
-      </c>
-      <c r="I12" s="48">
-        <v>5.16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="76" t="str">
+      <c r="H43" s="43">
+        <v>2.1</v>
+      </c>
+      <c r="I43" s="43">
+        <v>1</v>
+      </c>
+      <c r="J43" s="43">
+        <v>2.1</v>
+      </c>
+      <c r="K43" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>morbidity</v>
+      </c>
+      <c r="B44" s="69" t="str">
         <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="47" t="s">
+        <v>non-fatal</v>
+      </c>
+      <c r="C44" s="69" t="str">
+        <f t="shared" si="5"/>
+        <v>Diseases of the digestive system which can be caused caused by smoking</v>
+      </c>
+      <c r="D44" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" s="69">
+        <v>3</v>
+      </c>
+      <c r="F44" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="48">
-        <v>1</v>
-      </c>
-      <c r="G13" s="48">
-        <v>1</v>
-      </c>
-      <c r="H13" s="48">
-        <v>1.59</v>
-      </c>
-      <c r="I13" s="48">
+      <c r="H44" s="43">
+        <v>3.97</v>
+      </c>
+      <c r="I44" s="43">
+        <v>1.68</v>
+      </c>
+      <c r="J44" s="43">
+        <v>3.97</v>
+      </c>
+      <c r="K44" s="43">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+    </row>
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="78" t="str">
+        <f t="shared" si="0"/>
+        <v>non-fatal</v>
+      </c>
+      <c r="C46" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="78"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+    </row>
+    <row r="47" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>morbidity</v>
+      </c>
+      <c r="B47" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>non-fatal</v>
+      </c>
+      <c r="C47" s="69" t="str">
+        <f t="shared" ref="C47:C51" si="6">C46</f>
+        <v>Other diseases which can be caused by smoking</v>
+      </c>
+      <c r="D47" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" s="69">
+        <v>3</v>
+      </c>
+      <c r="F47" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="H47" s="43">
+        <v>1.54</v>
+      </c>
+      <c r="I47" s="43">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J47" s="43">
+        <v>1.54</v>
+      </c>
+      <c r="K47" s="43">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>morbidity</v>
+      </c>
+      <c r="B48" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>non-fatal</v>
+      </c>
+      <c r="C48" s="69" t="str">
+        <f t="shared" si="6"/>
+        <v>Other diseases which can be caused by smoking</v>
+      </c>
+      <c r="D48" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="E48" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="F48" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="G48" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="H48" s="43">
+        <v>1.17</v>
+      </c>
+      <c r="I48" s="43">
+        <v>1.02</v>
+      </c>
+      <c r="J48" s="43">
+        <v>1.17</v>
+      </c>
+      <c r="K48" s="43">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>morbidity</v>
+      </c>
+      <c r="B49" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>non-fatal</v>
+      </c>
+      <c r="C49" s="69" t="str">
+        <f t="shared" si="6"/>
+        <v>Other diseases which can be caused by smoking</v>
+      </c>
+      <c r="D49" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="E49" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="F49" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="G49" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H49" s="43">
+        <v>1.41</v>
+      </c>
+      <c r="I49" s="43">
+        <v>1.08</v>
+      </c>
+      <c r="J49" s="43">
+        <v>1.41</v>
+      </c>
+      <c r="K49" s="43">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="69" t="str">
+        <f t="shared" si="1"/>
+        <v>morbidity</v>
+      </c>
+      <c r="B50" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>non-fatal</v>
+      </c>
+      <c r="C50" s="69" t="str">
+        <f t="shared" si="6"/>
+        <v>Other diseases which can be caused by smoking</v>
+      </c>
+      <c r="D50" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="E50" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="F50" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="G50" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="H50" s="43">
+        <v>1.76</v>
+      </c>
+      <c r="I50" s="43">
         <v>1.1399999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="76" t="str">
+      <c r="J50" s="43">
+        <v>1.85</v>
+      </c>
+      <c r="K50" s="43">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A51" s="69" t="str">
+        <f>A50</f>
+        <v>morbidity</v>
+      </c>
+      <c r="B51" s="69" t="str">
         <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B14" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="47" t="s">
+        <v>non-fatal</v>
+      </c>
+      <c r="C51" s="69" t="str">
+        <f t="shared" si="6"/>
+        <v>Other diseases which can be caused by smoking</v>
+      </c>
+      <c r="D51" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" s="69">
+        <v>3</v>
+      </c>
+      <c r="F51" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="G51" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="48">
-        <v>3.27</v>
-      </c>
-      <c r="G14" s="48">
-        <v>2.09</v>
-      </c>
-      <c r="H14" s="48">
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="I14" s="48">
-        <v>1.89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="76" t="str">
-        <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B15" s="76" t="s">
-        <v>170</v>
-      </c>
-      <c r="C15" s="76">
-        <v>2</v>
-      </c>
-      <c r="D15" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="48">
-        <v>2.5</v>
-      </c>
-      <c r="G15" s="48">
-        <v>1.7</v>
-      </c>
-      <c r="H15" s="48">
-        <v>1.4</v>
-      </c>
-      <c r="I15" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="76" t="str">
-        <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B16" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="48">
-        <v>1.96</v>
-      </c>
-      <c r="G16" s="48">
-        <v>1.47</v>
-      </c>
-      <c r="H16" s="48">
-        <v>1.36</v>
-      </c>
-      <c r="I16" s="48">
-        <v>1.32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="76" t="str">
-        <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="48">
-        <v>2.31</v>
-      </c>
-      <c r="G17" s="48">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="H17" s="48">
-        <v>2.25</v>
-      </c>
-      <c r="I17" s="48">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="76" t="str">
-        <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B18" s="76" t="s">
-        <v>171</v>
-      </c>
-      <c r="C18" s="76">
-        <v>2</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="48">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G18" s="48">
-        <v>2.5</v>
-      </c>
-      <c r="H18" s="48">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I18" s="48">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="76" t="str">
-        <f t="shared" si="0"/>
-        <v>Cancers which can be caused by smoking</v>
-      </c>
-      <c r="B19" s="76" t="s">
-        <v>172</v>
-      </c>
-      <c r="C19" s="76">
-        <v>2</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="48">
-        <v>1.8</v>
-      </c>
-      <c r="G19" s="48">
-        <v>1.4</v>
-      </c>
-      <c r="H19" s="48">
-        <v>1.2</v>
-      </c>
-      <c r="I19" s="48">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="50"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="87"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-    </row>
-    <row r="22" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="76" t="str">
-        <f t="shared" ref="A22:A25" si="1">A21</f>
-        <v>Respiratory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B22" s="50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="50"/>
-      <c r="D22" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="48">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="G22" s="48">
-        <v>15.64</v>
-      </c>
-      <c r="H22" s="48">
-        <v>12.04</v>
-      </c>
-      <c r="I22" s="48">
-        <v>11.77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="76" t="str">
-        <f t="shared" si="1"/>
-        <v>Respiratory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B23" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="48">
-        <v>10.58</v>
-      </c>
-      <c r="G23" s="48">
-        <v>6.8</v>
-      </c>
-      <c r="H23" s="48">
-        <v>13.08</v>
-      </c>
-      <c r="I23" s="48">
-        <v>6.78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="76" t="str">
-        <f t="shared" si="1"/>
-        <v>Respiratory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B24" s="76" t="s">
-        <v>159</v>
-      </c>
-      <c r="C24" s="76">
-        <v>2</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="48">
-        <v>2.5</v>
-      </c>
-      <c r="G24" s="48">
-        <v>1.4</v>
-      </c>
-      <c r="H24" s="48">
-        <v>4.3</v>
-      </c>
-      <c r="I24" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="76" t="str">
-        <f t="shared" si="1"/>
-        <v>Respiratory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B25" s="76" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="76">
-        <v>2</v>
-      </c>
-      <c r="D25" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="48">
-        <v>2</v>
-      </c>
-      <c r="G25" s="48">
-        <v>1.4</v>
-      </c>
-      <c r="H25" s="48">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I25" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="B27" s="87"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-    </row>
-    <row r="28" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="76" t="str">
-        <f t="shared" ref="A28:A39" si="2">A27</f>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B28" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="48">
-        <v>1.78</v>
-      </c>
-      <c r="G28" s="48">
-        <v>1.22</v>
-      </c>
-      <c r="H28" s="48">
-        <v>1.49</v>
-      </c>
-      <c r="I28" s="48">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B29" s="76" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" s="76">
-        <v>2</v>
-      </c>
-      <c r="D29" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="48">
-        <v>4.2</v>
-      </c>
-      <c r="G29" s="48">
-        <v>2</v>
-      </c>
-      <c r="H29" s="48">
-        <v>5.3</v>
-      </c>
-      <c r="I29" s="48">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B30" s="76" t="s">
-        <v>158</v>
-      </c>
-      <c r="C30" s="76">
-        <v>2</v>
-      </c>
-      <c r="D30" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="F30" s="48">
-        <v>2.5</v>
-      </c>
-      <c r="G30" s="48">
-        <v>1.6</v>
-      </c>
-      <c r="H30" s="48">
-        <v>2.8</v>
-      </c>
-      <c r="I30" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B31" s="76" t="s">
-        <v>158</v>
-      </c>
-      <c r="C31" s="76">
-        <v>2</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="E31" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" s="48">
-        <v>1.8</v>
-      </c>
-      <c r="G31" s="48">
-        <v>1.3</v>
-      </c>
-      <c r="H31" s="48">
-        <v>2.1</v>
-      </c>
-      <c r="I31" s="48">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B32" s="76" t="s">
-        <v>158</v>
-      </c>
-      <c r="C32" s="76">
-        <v>2</v>
-      </c>
-      <c r="D32" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="48">
-        <v>1.4</v>
-      </c>
-      <c r="G32" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H32" s="48">
-        <v>1.4</v>
-      </c>
-      <c r="I32" s="48">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B33" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="48">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="G33" s="48">
-        <v>1.01</v>
-      </c>
-      <c r="H33" s="48">
-        <v>2.17</v>
-      </c>
-      <c r="I33" s="48">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B34" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="C34" s="76">
-        <v>2</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="E34" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="48">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G34" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H34" s="48">
-        <v>5.4</v>
-      </c>
-      <c r="I34" s="48">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B35" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="C35" s="76">
-        <v>2</v>
-      </c>
-      <c r="D35" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" s="48">
-        <v>3.1</v>
-      </c>
-      <c r="G35" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H35" s="48">
-        <v>3.7</v>
-      </c>
-      <c r="I35" s="48">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B36" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="C36" s="76">
-        <v>2</v>
-      </c>
-      <c r="D36" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="E36" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" s="48">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G36" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H36" s="48">
-        <v>2.6</v>
-      </c>
-      <c r="I36" s="48">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A37" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B37" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="C37" s="76">
-        <v>2</v>
-      </c>
-      <c r="D37" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" s="48">
-        <v>1.6</v>
-      </c>
-      <c r="G37" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H37" s="48">
-        <v>1.3</v>
-      </c>
-      <c r="I37" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A38" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B38" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="50"/>
-      <c r="D38" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F38" s="48">
-        <v>6.21</v>
-      </c>
-      <c r="G38" s="48">
-        <v>3.07</v>
-      </c>
-      <c r="H38" s="48">
-        <v>7.07</v>
-      </c>
-      <c r="I38" s="48">
-        <v>2.0699999999999998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="76" t="str">
-        <f t="shared" si="2"/>
-        <v>Circulatory diseases which can be caused by smoking</v>
-      </c>
-      <c r="B39" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="50"/>
-      <c r="D39" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="E39" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" s="48">
-        <v>2.44</v>
-      </c>
-      <c r="G39" s="48">
-        <v>1.33</v>
-      </c>
-      <c r="H39" s="48">
-        <v>1.83</v>
-      </c>
-      <c r="I39" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="50"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-    </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="88" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="89"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-    </row>
-    <row r="42" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="76" t="str">
-        <f t="shared" ref="A42:A44" si="3">A41</f>
-        <v>Diseases of the digestive system which can be caused caused by smoking</v>
-      </c>
-      <c r="B42" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" s="51"/>
-      <c r="D42" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="48">
-        <v>5.4</v>
-      </c>
-      <c r="G42" s="48">
-        <v>1.8</v>
-      </c>
-      <c r="H42" s="48">
-        <v>5.5</v>
-      </c>
-      <c r="I42" s="48">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="76" t="str">
-        <f t="shared" si="3"/>
-        <v>Diseases of the digestive system which can be caused caused by smoking</v>
-      </c>
-      <c r="B43" s="76" t="s">
-        <v>160</v>
-      </c>
-      <c r="C43" s="76">
-        <v>3</v>
-      </c>
-      <c r="D43" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" s="48">
-        <v>2.1</v>
-      </c>
-      <c r="G43" s="48">
-        <v>1</v>
-      </c>
-      <c r="H43" s="48">
-        <v>2.1</v>
-      </c>
-      <c r="I43" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="76" t="str">
-        <f t="shared" si="3"/>
-        <v>Diseases of the digestive system which can be caused caused by smoking</v>
-      </c>
-      <c r="B44" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="C44" s="76">
-        <v>3</v>
-      </c>
-      <c r="D44" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F44" s="48">
-        <v>3.97</v>
-      </c>
-      <c r="G44" s="48">
-        <v>1.68</v>
-      </c>
-      <c r="H44" s="48">
-        <v>3.97</v>
-      </c>
-      <c r="I44" s="48">
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="50"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="87"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-    </row>
-    <row r="47" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="76" t="str">
-        <f t="shared" ref="A47:A51" si="4">A46</f>
-        <v>Other diseases which can be caused by smoking</v>
-      </c>
-      <c r="B47" s="76" t="s">
-        <v>162</v>
-      </c>
-      <c r="C47" s="76">
-        <v>3</v>
-      </c>
-      <c r="D47" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="F47" s="48">
-        <v>1.54</v>
-      </c>
-      <c r="G47" s="48">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="H47" s="48">
-        <v>1.54</v>
-      </c>
-      <c r="I47" s="48">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="76" t="str">
-        <f t="shared" si="4"/>
-        <v>Other diseases which can be caused by smoking</v>
-      </c>
-      <c r="B48" s="76" t="s">
-        <v>163</v>
-      </c>
-      <c r="C48" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="D48" s="77" t="s">
-        <v>166</v>
-      </c>
-      <c r="E48" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="F48" s="48">
-        <v>1.17</v>
-      </c>
-      <c r="G48" s="48">
-        <v>1.02</v>
-      </c>
-      <c r="H48" s="48">
-        <v>1.17</v>
-      </c>
-      <c r="I48" s="48">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="76" t="str">
-        <f t="shared" si="4"/>
-        <v>Other diseases which can be caused by smoking</v>
-      </c>
-      <c r="B49" s="76" t="s">
-        <v>163</v>
-      </c>
-      <c r="C49" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="D49" s="77" t="s">
-        <v>166</v>
-      </c>
-      <c r="E49" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="F49" s="48">
-        <v>1.41</v>
-      </c>
-      <c r="G49" s="48">
-        <v>1.08</v>
-      </c>
-      <c r="H49" s="48">
-        <v>1.41</v>
-      </c>
-      <c r="I49" s="48">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="76" t="str">
-        <f t="shared" si="4"/>
-        <v>Other diseases which can be caused by smoking</v>
-      </c>
-      <c r="B50" s="76" t="s">
-        <v>163</v>
-      </c>
-      <c r="C50" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="D50" s="77" t="s">
-        <v>166</v>
-      </c>
-      <c r="E50" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="F50" s="48">
-        <v>1.76</v>
-      </c>
-      <c r="G50" s="48">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="H50" s="48">
-        <v>1.85</v>
-      </c>
-      <c r="I50" s="48">
-        <v>1.22</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A51" s="76" t="str">
-        <f t="shared" si="4"/>
-        <v>Other diseases which can be caused by smoking</v>
-      </c>
-      <c r="B51" s="76" t="s">
-        <v>164</v>
-      </c>
-      <c r="C51" s="76">
-        <v>3</v>
-      </c>
-      <c r="D51" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="E51" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48">
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43">
         <v>1.28</v>
       </c>
-      <c r="I51" s="48"/>
-    </row>
-    <row r="52" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A52" s="57"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="59"/>
-    </row>
-    <row r="53" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="60"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
-      <c r="H53" s="61"/>
-      <c r="I53" s="61"/>
-    </row>
-    <row r="54" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A54" s="60"/>
-      <c r="B54" s="60" t="s">
+      <c r="K51" s="43"/>
+    </row>
+    <row r="52" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A52" s="52"/>
+      <c r="B52" s="52"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="54"/>
+      <c r="I52" s="54"/>
+      <c r="J52" s="54"/>
+      <c r="K52" s="54"/>
+    </row>
+    <row r="53" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="55"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="56"/>
+    </row>
+    <row r="54" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A54" s="55"/>
+      <c r="B54" s="55"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="C54" s="60"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="61"/>
-      <c r="H54" s="61"/>
-      <c r="I54" s="61"/>
-    </row>
-    <row r="55" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A55" s="60"/>
-      <c r="B55" s="60"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="61"/>
-      <c r="G55" s="61"/>
-      <c r="H55" s="61"/>
-      <c r="I55" s="61"/>
-    </row>
-    <row r="56" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A56" s="62"/>
-      <c r="B56" s="62" t="s">
+      <c r="E54" s="55"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="56"/>
+      <c r="I54" s="56"/>
+      <c r="J54" s="56"/>
+      <c r="K54" s="56"/>
+    </row>
+    <row r="55" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A55" s="55"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="56"/>
+      <c r="I55" s="56"/>
+      <c r="J55" s="56"/>
+      <c r="K55" s="56"/>
+    </row>
+    <row r="56" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A56" s="57"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="57"/>
+      <c r="D56" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="62"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="48"/>
-    </row>
-    <row r="57" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="41"/>
-      <c r="B57" s="41" t="s">
+      <c r="E56" s="57"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
+    </row>
+    <row r="57" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="48"/>
-    </row>
-    <row r="58" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A58" s="41"/>
-      <c r="B58" s="41" t="s">
+      <c r="E57" s="37"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="43"/>
+    </row>
+    <row r="58" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A58" s="37"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="41"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="48"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="48"/>
-      <c r="I58" s="48"/>
-    </row>
-    <row r="59" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="41"/>
-      <c r="B59" s="41" t="s">
+      <c r="E58" s="37"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
+      <c r="H58" s="43"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="43"/>
+      <c r="K58" s="43"/>
+    </row>
+    <row r="59" spans="1:11" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="41"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="41"/>
-      <c r="B60" s="41" t="s">
+      <c r="E59" s="37"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="42"/>
+      <c r="H59" s="43"/>
+      <c r="I59" s="43"/>
+      <c r="J59" s="43"/>
+      <c r="K59" s="43"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="37"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C60" s="41"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="41"/>
-      <c r="B61" s="41"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="41"/>
-      <c r="E61" s="41"/>
-      <c r="F61" s="41"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="41"/>
-      <c r="I61" s="41"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="62"/>
-      <c r="B62" s="62" t="s">
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="37"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="57"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C62" s="62"/>
-      <c r="D62" s="41"/>
-      <c r="E62" s="41"/>
-      <c r="F62" s="41"/>
-      <c r="G62" s="41"/>
-      <c r="H62" s="41"/>
-      <c r="I62" s="41"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="41"/>
-      <c r="B63" s="41" t="s">
+      <c r="E62" s="57"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="37"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="41"/>
-      <c r="F63" s="41"/>
-      <c r="G63" s="41"/>
-      <c r="H63" s="41"/>
-      <c r="I63" s="41"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="41"/>
-      <c r="B64" s="41" t="s">
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
-      <c r="F64" s="41"/>
-      <c r="G64" s="41"/>
-      <c r="H64" s="41"/>
-      <c r="I64" s="41"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="41"/>
-      <c r="B65" s="41"/>
-      <c r="C65" s="41"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="41"/>
-      <c r="F65" s="41"/>
-      <c r="G65" s="41"/>
-      <c r="H65" s="41"/>
-      <c r="I65" s="41"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="41"/>
-      <c r="B66" s="41" t="s">
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="37"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="41"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="41"/>
-      <c r="I66" s="41"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="41"/>
-      <c r="B67" s="41" t="s">
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
+      <c r="K66" s="37"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="41"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="41"/>
-      <c r="G67" s="41"/>
-      <c r="H67" s="41"/>
-      <c r="I67" s="41"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
@@ -4778,167 +5144,165 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F831F7E-E642-4D51-B145-13F003379413}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="68" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" s="75" t="s">
+      <c r="D7" s="68" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="75" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="75" t="s">
+      <c r="F7" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="68" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="73">
+      <c r="B8" s="65"/>
+      <c r="C8" s="66">
         <v>1</v>
       </c>
-      <c r="D8" s="73">
+      <c r="D8" s="66">
         <v>1</v>
       </c>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="73">
+      <c r="B9" s="65"/>
+      <c r="C9" s="66">
         <v>1</v>
       </c>
-      <c r="D9" s="73">
+      <c r="D9" s="66">
         <v>1</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="66">
         <v>1</v>
       </c>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="73">
+      <c r="B10" s="65"/>
+      <c r="C10" s="66">
         <v>1</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="66">
         <v>1</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="66">
         <v>1</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="66">
         <v>1</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G10" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73">
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66">
         <v>1</v>
       </c>
-      <c r="E11" s="73">
+      <c r="E11" s="66">
         <v>1</v>
       </c>
-      <c r="F11" s="73">
+      <c r="F11" s="66">
         <v>1</v>
       </c>
-      <c r="G11" s="73">
+      <c r="G11" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="72"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73">
+      <c r="B12" s="65"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66">
         <v>1</v>
       </c>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73">
+      <c r="B13" s="65"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66">
         <v>1</v>
       </c>
-      <c r="G13" s="73"/>
+      <c r="G13" s="66"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73">
+      <c r="B14" s="65"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66">
         <v>1</v>
       </c>
-      <c r="G14" s="73">
+      <c r="G14" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="71" t="s">
+      <c r="A15" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="72"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73">
+      <c r="B15" s="65"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66">
         <v>1</v>
       </c>
     </row>

</xml_diff>